<commit_message>
bi: update couverture forms
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burundi/2022 October/bi_couverture_2_couverture_202210.xlsx
+++ b/Coverage Survey/Burundi/2022 October/bi_couverture_2_couverture_202210.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="233">
   <si>
     <t>type</t>
   </si>
@@ -492,6 +492,9 @@
     <t>1.Voyage</t>
   </si>
   <si>
+    <t>2. A l.internat /Ecole</t>
+  </si>
+  <si>
     <t>2. A l'internat /Ecole</t>
   </si>
   <si>
@@ -507,6 +510,9 @@
     <t>non_menage_enr</t>
   </si>
   <si>
+    <t>1. DC/ASC n.est pas venu</t>
+  </si>
+  <si>
     <t>1. DC/ASC n'est pas venu</t>
   </si>
   <si>
@@ -516,6 +522,9 @@
     <t xml:space="preserve">3. Absent pendant le jour de campagne </t>
   </si>
   <si>
+    <t xml:space="preserve">4. Personne n.était à la maison </t>
+  </si>
+  <si>
     <t xml:space="preserve">4. Personne n'était à la maison </t>
   </si>
   <si>
@@ -600,7 +609,7 @@
     <t>3. Je ne suis pas malade</t>
   </si>
   <si>
-    <t>4.pas.recu.suffisamment.d’informations</t>
+    <t>4.pas.recu.suffisamment.d.informations</t>
   </si>
   <si>
     <t xml:space="preserve">4. Je n'ai pas eu suffisament d'informations sur le médicament </t>
@@ -1854,7 +1863,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E$1:E$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="12.75"/>
@@ -3227,9 +3236,9 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -3339,7 +3348,7 @@
         <v>158</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3347,10 +3356,10 @@
         <v>156</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3358,10 +3367,10 @@
         <v>156</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3369,10 +3378,10 @@
         <v>156</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3382,57 +3391,57 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>161</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3442,7 +3451,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>152</v>
@@ -3453,7 +3462,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>154</v>
@@ -3464,13 +3473,13 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3480,101 +3489,101 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3584,57 +3593,57 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -3644,57 +3653,57 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -3704,123 +3713,123 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B47" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C47" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C51" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C53" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C54" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C55" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C56" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3854,25 +3863,25 @@
   <sheetData>
     <row r="1" ht="14.25" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D2" s="3"/>
     </row>

</xml_diff>